<commit_message>
Preparar Excels para Bots de recibos
</commit_message>
<xml_diff>
--- a/Archivo para hacer Facturas 3.0 YYYY.xlsx
+++ b/Archivo para hacer Facturas 3.0 YYYY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\BOT-Facturador-AFIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C2C418-B618-4260-8471-070848181FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AB9936-2BB7-4EBA-8AD8-94BAA138853B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1216,7 +1216,7 @@
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="K17" sqref="K17"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1391,15 +1391,15 @@
         <v>45084</v>
       </c>
       <c r="B2" s="9" t="e">
-        <f ca="1">TEXT(DATE(YEAR(C2),MONTH(C2),1),"dd/mm/YYYY")</f>
+        <f t="shared" ref="B2:B17" ca="1" si="0">TEXT(DATE(YEAR(C2),MONTH(C2),1),"dd/mm/YYYY")</f>
         <v>#VALUE!</v>
       </c>
       <c r="C2" s="9" t="str">
-        <f ca="1">TEXT(EOMONTH(A2,-1),"dd/mm/YYYY")</f>
+        <f t="shared" ref="C2:C17" ca="1" si="1">TEXT(EOMONTH(A2,-1),"dd/mm/YYYY")</f>
         <v>31/05/YYYY</v>
       </c>
       <c r="D2" s="9" t="str">
-        <f ca="1">TEXT(A2+14,"dd/mm/YYYY")</f>
+        <f t="shared" ref="D2:D17" ca="1" si="2">TEXT(A2+14,"dd/mm/YYYY")</f>
         <v>21/06/YYYY</v>
       </c>
       <c r="E2" s="2">
@@ -1448,7 +1448,7 @@
         <v>2</v>
       </c>
       <c r="V2" s="18" t="str">
-        <f t="shared" ref="V2:V17" si="0">SUBSTITUTE(IF(AJ2="A",ROUND(O2/N2,6),ROUND(AB2/N2,6)),",",".")</f>
+        <f t="shared" ref="V2:V17" si="3">SUBSTITUTE(IF(AJ2="A",ROUND(O2/N2,6),ROUND(AB2/N2,6)),",",".")</f>
         <v>7.003044</v>
       </c>
       <c r="W2" s="18" t="str">
@@ -1456,19 +1456,19 @@
         <v>19000.00</v>
       </c>
       <c r="X2" s="1" t="str">
-        <f t="shared" ref="X2:X17" si="1">TEXT(R2,"00000")</f>
+        <f t="shared" ref="X2:X17" si="4">TEXT(R2,"00000")</f>
         <v>00000</v>
       </c>
       <c r="Y2" s="1" t="str">
-        <f t="shared" ref="Y2:Y17" si="2">TEXT(S2,"00000000")</f>
+        <f t="shared" ref="Y2:Y17" si="5">TEXT(S2,"00000000")</f>
         <v>00000000</v>
       </c>
       <c r="Z2" s="1" t="str">
-        <f>TEXT(T2,"DD/MM/YYYY")</f>
+        <f t="shared" ref="Z2:Z17" si="6">TEXT(T2,"DD/MM/YYYY")</f>
         <v>00/01/YYYY</v>
       </c>
       <c r="AA2" s="13">
-        <f t="shared" ref="AA2:AA17" si="3">IF(AJ2="A",ROUND(O2*P2,2),ROUND(O2*P2/(1+P2),2))</f>
+        <f t="shared" ref="AA2:AA17" si="7">IF(AJ2="A",ROUND(O2*P2,2),ROUND(O2*P2/(1+P2),2))</f>
         <v>27942.15</v>
       </c>
       <c r="AB2" s="13">
@@ -1476,7 +1476,7 @@
         <v>160999.99</v>
       </c>
       <c r="AC2" s="10" t="str">
-        <f t="shared" ref="AC2:AC17" si="4">IF(RIGHT(F2,1)="A",SUBSTITUTE(TEXT(O2,"0,00"),",","."),SUBSTITUTE(TEXT(AB2,"0,00"),",","."))</f>
+        <f t="shared" ref="AC2:AC17" si="8">IF(RIGHT(F2,1)="A",SUBSTITUTE(TEXT(O2,"0,00"),",","."),SUBSTITUTE(TEXT(AB2,"0,00"),",","."))</f>
         <v>133057.84</v>
       </c>
       <c r="AD2" s="10" t="str">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1">
-        <f t="shared" ref="AF2:AF17" si="5">ROW(K2)</f>
+        <f t="shared" ref="AF2:AF17" si="9">ROW(K2)</f>
         <v>2</v>
       </c>
       <c r="AG2" s="15" t="str">
@@ -1493,19 +1493,19 @@
         <v>30525390086-1</v>
       </c>
       <c r="AH2" s="1">
-        <f t="shared" ref="AH2:AH17" si="6">IF(K1=K2,1,0)</f>
+        <f t="shared" ref="AH2:AH17" si="10">IF(K1=K2,1,0)</f>
         <v>0</v>
       </c>
       <c r="AI2" s="1">
-        <f t="shared" ref="AI2:AI17" si="7">IF(K2=K3,1,0)</f>
+        <f t="shared" ref="AI2:AI17" si="11">IF(K2=K3,1,0)</f>
         <v>0</v>
       </c>
       <c r="AJ2" s="1" t="str">
-        <f t="shared" ref="AJ2:AJ17" si="8">RIGHT(F2)</f>
+        <f t="shared" ref="AJ2:AJ17" si="12">RIGHT(F2)</f>
         <v>A</v>
       </c>
       <c r="AK2" s="1">
-        <f>IF(LEFT(F2,4)="Nota",0,1)</f>
+        <f t="shared" ref="AK2:AK17" si="13">IF(LEFT(F2,4)="Nota",0,IF(LEFT(F2,6)="Recibo",2,1))</f>
         <v>1</v>
       </c>
       <c r="AL2" s="2"/>
@@ -1514,15 +1514,15 @@
         <v>160999.98000000001</v>
       </c>
       <c r="AN2" s="13">
-        <f t="shared" ref="AN2:AN17" si="9">ROUND((AM2/(1+P2)),2)</f>
+        <f t="shared" ref="AN2:AN17" si="14">ROUND((AM2/(1+P2)),2)</f>
         <v>133057.82999999999</v>
       </c>
       <c r="AO2" s="20">
-        <f t="shared" ref="AO2:AO17" si="10">IF(AJ2="A",ROUND(AN2/N2,6),AM2/N2)</f>
+        <f t="shared" ref="AO2:AO17" si="15">IF(AJ2="A",ROUND(AN2/N2,6),AM2/N2)</f>
         <v>7.003044</v>
       </c>
       <c r="AP2" s="13">
-        <f t="shared" ref="AP2:AP17" si="11">IF(AJ2="A",ROUND(CEILING(N2*M2*(1+P2),500),2),ROUND(CEILING(N2*M2,500),2))</f>
+        <f t="shared" ref="AP2:AP17" si="16">IF(AJ2="A",ROUND(CEILING(N2*M2*(1+P2),500),2),ROUND(CEILING(N2*M2,500),2))</f>
         <v>161000</v>
       </c>
       <c r="AQ2" s="20">
@@ -1533,19 +1533,19 @@
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <f t="shared" ref="A3:A17" ca="1" si="12">TODAY()</f>
+        <f t="shared" ref="A3:A17" ca="1" si="17">TODAY()</f>
         <v>45084</v>
       </c>
       <c r="B3" s="9" t="e">
-        <f ca="1">TEXT(DATE(YEAR(C3),MONTH(C3),1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="C3" s="9" t="str">
-        <f ca="1">TEXT(EOMONTH(A3,-1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>31/05/YYYY</v>
       </c>
       <c r="D3" s="9" t="str">
-        <f ca="1">TEXT(A3+14,"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>21/06/YYYY</v>
       </c>
       <c r="E3" s="2">
@@ -1580,7 +1580,7 @@
         <v>19000</v>
       </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O17" si="13">M3*N3</f>
+        <f t="shared" ref="O3:O17" si="18">M3*N3</f>
         <v>152479.33199999999</v>
       </c>
       <c r="P3" s="11" t="s">
@@ -1595,35 +1595,35 @@
         <v>2</v>
       </c>
       <c r="V3" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>8.025228</v>
       </c>
       <c r="W3" s="18" t="str">
-        <f t="shared" ref="W3:W17" si="14">SUBSTITUTE(TEXT(N3,"0,00"),",",".")</f>
+        <f t="shared" ref="W3:W17" si="19">SUBSTITUTE(TEXT(N3,"0,00"),",",".")</f>
         <v>19000.00</v>
       </c>
       <c r="X3" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y3" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z3" s="1" t="str">
-        <f>TEXT(T3,"DD/MM/YYYY")</f>
+        <f t="shared" si="6"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="AA3" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>32020.66</v>
       </c>
       <c r="AB3" s="13">
-        <f t="shared" ref="AB3:AB17" si="15">IF(AJ3="A",ROUND(O3+AA3,2),ROUND(O3,2))</f>
+        <f t="shared" ref="AB3:AB17" si="20">IF(AJ3="A",ROUND(O3+AA3,2),ROUND(O3,2))</f>
         <v>184499.99</v>
       </c>
       <c r="AC3" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>152479.33</v>
       </c>
       <c r="AD3" s="10" t="str">
@@ -1632,7 +1632,7 @@
       </c>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="AG3" s="15" t="str">
@@ -1640,59 +1640,59 @@
         <v>30525733870-1</v>
       </c>
       <c r="AH3" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI3" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ3" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK3" s="1">
-        <f t="shared" ref="AK3:AK17" si="16">IF(LEFT(F3,4)="Nota",0,1)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AL3" s="2"/>
       <c r="AM3" s="13">
-        <f t="shared" ref="AM3:AM17" si="17">IF(RIGHT(F3,1)="A",ROUND(N3*M3*(1+P3),2),AB3)</f>
+        <f t="shared" ref="AM3:AM17" si="21">IF(RIGHT(F3,1)="A",ROUND(N3*M3*(1+P3),2),AB3)</f>
         <v>184499.99</v>
       </c>
       <c r="AN3" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>152479.32999999999</v>
       </c>
       <c r="AO3" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>8.0252280000000003</v>
       </c>
       <c r="AP3" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>184500</v>
       </c>
       <c r="AQ3" s="20">
-        <f t="shared" ref="AQ3:AQ17" si="18">IF(AJ3="A",ROUND(AN3/N3,6),AP3/N3)</f>
+        <f t="shared" ref="AQ3:AQ17" si="22">IF(AJ3="A",ROUND(AN3/N3,6),AP3/N3)</f>
         <v>8.0252280000000003</v>
       </c>
       <c r="AR3" s="2"/>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="17"/>
         <v>45084</v>
       </c>
       <c r="B4" s="9" t="e">
-        <f ca="1">TEXT(DATE(YEAR(C4),MONTH(C4),1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="C4" s="9" t="str">
-        <f ca="1">TEXT(EOMONTH(A4,-1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>31/05/YYYY</v>
       </c>
       <c r="D4" s="9" t="str">
-        <f ca="1">TEXT(A4+14,"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>21/06/YYYY</v>
       </c>
       <c r="E4" s="2">
@@ -1727,7 +1727,7 @@
         <v>19000</v>
       </c>
       <c r="O4" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>190082.63099999999</v>
       </c>
       <c r="P4" s="11" t="s">
@@ -1742,35 +1742,35 @@
         <v>2</v>
       </c>
       <c r="V4" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>10.004349</v>
       </c>
       <c r="W4" s="18" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>19000.00</v>
       </c>
       <c r="X4" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y4" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z4" s="1" t="str">
-        <f>TEXT(T4,"DD/MM/YYYY")</f>
+        <f t="shared" si="6"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="AA4" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>39917.35</v>
       </c>
       <c r="AB4" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>229999.98</v>
       </c>
       <c r="AC4" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>190082.63</v>
       </c>
       <c r="AD4" s="10" t="str">
@@ -1779,7 +1779,7 @@
       </c>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AG4" s="15" t="str">
@@ -1787,59 +1787,59 @@
         <v>30610252334-1</v>
       </c>
       <c r="AH4" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI4" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ4" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK4" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AL4" s="2"/>
       <c r="AM4" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>229999.98</v>
       </c>
       <c r="AN4" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>190082.63</v>
       </c>
       <c r="AO4" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>10.004348999999999</v>
       </c>
       <c r="AP4" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>230000</v>
       </c>
       <c r="AQ4" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>10.004348999999999</v>
       </c>
       <c r="AR4" s="2"/>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="17"/>
         <v>45084</v>
       </c>
       <c r="B5" s="9" t="e">
-        <f ca="1">TEXT(DATE(YEAR(C5),MONTH(C5),1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="C5" s="9" t="str">
-        <f ca="1">TEXT(EOMONTH(A5,-1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>31/05/YYYY</v>
       </c>
       <c r="D5" s="9" t="str">
-        <f ca="1">TEXT(A5+14,"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>21/06/YYYY</v>
       </c>
       <c r="E5" s="2">
@@ -1874,7 +1874,7 @@
         <v>19000</v>
       </c>
       <c r="O5" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>171487.59700000001</v>
       </c>
       <c r="P5" s="11" t="s">
@@ -1889,35 +1889,35 @@
         <v>2</v>
       </c>
       <c r="V5" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9.025663</v>
       </c>
       <c r="W5" s="18" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>19000.00</v>
       </c>
       <c r="X5" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y5" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z5" s="1" t="str">
-        <f>TEXT(T5,"DD/MM/YYYY")</f>
+        <f t="shared" si="6"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="AA5" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>36012.400000000001</v>
       </c>
       <c r="AB5" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>207500</v>
       </c>
       <c r="AC5" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>171487.60</v>
       </c>
       <c r="AD5" s="10" t="str">
@@ -1926,7 +1926,7 @@
       </c>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AG5" s="15" t="str">
@@ -1934,59 +1934,59 @@
         <v>30710964277-1</v>
       </c>
       <c r="AH5" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI5" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ5" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK5" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AL5" s="2"/>
       <c r="AM5" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>207499.99</v>
       </c>
       <c r="AN5" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>171487.6</v>
       </c>
       <c r="AO5" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>9.0256629999999998</v>
       </c>
       <c r="AP5" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>207500</v>
       </c>
       <c r="AQ5" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>9.0256629999999998</v>
       </c>
       <c r="AR5" s="2"/>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="17"/>
         <v>45084</v>
       </c>
       <c r="B6" s="9" t="e">
-        <f ca="1">TEXT(DATE(YEAR(C6),MONTH(C6),1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="C6" s="9" t="str">
-        <f ca="1">TEXT(EOMONTH(A6,-1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>31/05/YYYY</v>
       </c>
       <c r="D6" s="9" t="str">
-        <f ca="1">TEXT(A6+14,"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>21/06/YYYY</v>
       </c>
       <c r="E6" s="2">
@@ -2021,7 +2021,7 @@
         <v>19000</v>
       </c>
       <c r="O6" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>95454.536999999997</v>
       </c>
       <c r="P6" s="11" t="s">
@@ -2044,35 +2044,35 @@
         <v>2</v>
       </c>
       <c r="V6" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5.023923</v>
       </c>
       <c r="W6" s="18" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>19000.00</v>
       </c>
       <c r="X6" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>00002</v>
       </c>
       <c r="Y6" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>00000003</v>
       </c>
       <c r="Z6" s="1" t="str">
-        <f>TEXT(T6,"DD/MM/YYYY")</f>
+        <f t="shared" si="6"/>
         <v>12/09/YYYY</v>
       </c>
       <c r="AA6" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>20045.45</v>
       </c>
       <c r="AB6" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>115499.99</v>
       </c>
       <c r="AC6" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>95454.54</v>
       </c>
       <c r="AD6" s="10" t="str">
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AG6" s="15" t="str">
@@ -2089,59 +2089,59 @@
         <v>33610006189-1</v>
       </c>
       <c r="AH6" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI6" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="AJ6" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK6" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AL6" s="2"/>
       <c r="AM6" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>115499.99</v>
       </c>
       <c r="AN6" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>95454.54</v>
       </c>
       <c r="AO6" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>5.0239229999999999</v>
       </c>
       <c r="AP6" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>115500</v>
       </c>
       <c r="AQ6" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>5.0239229999999999</v>
       </c>
       <c r="AR6" s="2"/>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="17"/>
         <v>45084</v>
       </c>
       <c r="B7" s="9" t="e">
-        <f ca="1">TEXT(DATE(YEAR(C7),MONTH(C7),1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="C7" s="9" t="str">
-        <f ca="1">TEXT(EOMONTH(A7,-1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>31/05/YYYY</v>
       </c>
       <c r="D7" s="9" t="str">
-        <f ca="1">TEXT(A7+14,"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>21/06/YYYY</v>
       </c>
       <c r="E7" s="2">
@@ -2175,7 +2175,7 @@
         <v>19000</v>
       </c>
       <c r="O7" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>95041.305999999997</v>
       </c>
       <c r="P7" s="11" t="s">
@@ -2190,44 +2190,44 @@
         <v>3</v>
       </c>
       <c r="V7" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5.002174</v>
       </c>
       <c r="W7" s="18" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>19000.00</v>
       </c>
       <c r="X7" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y7" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z7" s="1" t="str">
-        <f>TEXT(T7,"DD/MM/YYYY")</f>
+        <f t="shared" si="6"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="AA7" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>19958.669999999998</v>
       </c>
       <c r="AB7" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>114999.98</v>
       </c>
       <c r="AC7" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>95041.31</v>
       </c>
       <c r="AD7" s="10" t="str">
-        <f t="shared" ref="AD7:AD17" si="19">SUBSTITUTE(TEXT(ROUNDUP(AB7,0)-AB7,"0,00"),",",".")</f>
+        <f t="shared" ref="AD7:AD17" si="23">SUBSTITUTE(TEXT(ROUNDUP(AB7,0)-AB7,"0,00"),",",".")</f>
         <v>0.02</v>
       </c>
       <c r="AE7" s="1"/>
       <c r="AF7" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AG7" s="15" t="str">
@@ -2235,59 +2235,59 @@
         <v>33610006189-2</v>
       </c>
       <c r="AH7" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="AI7" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ7" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK7" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AL7" s="2"/>
       <c r="AM7" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>114999.98</v>
       </c>
       <c r="AN7" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>95041.31</v>
       </c>
       <c r="AO7" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>5.0021740000000001</v>
       </c>
       <c r="AP7" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>115000</v>
       </c>
       <c r="AQ7" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>5.0021740000000001</v>
       </c>
       <c r="AR7" s="2"/>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="17"/>
         <v>45084</v>
       </c>
       <c r="B8" s="9" t="e">
-        <f ca="1">TEXT(DATE(YEAR(C8),MONTH(C8),1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="C8" s="9" t="str">
-        <f ca="1">TEXT(EOMONTH(A8,-1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>31/05/YYYY</v>
       </c>
       <c r="D8" s="9" t="str">
-        <f ca="1">TEXT(A8+14,"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>21/06/YYYY</v>
       </c>
       <c r="E8" s="2">
@@ -2312,7 +2312,7 @@
         <v>52</v>
       </c>
       <c r="L8" s="1" t="e">
-        <f t="shared" ref="L8:L13" ca="1" si="20">"Honorarios "&amp;PROPER(TEXT(B8,"mmmm"))</f>
+        <f t="shared" ref="L8:L13" ca="1" si="24">"Honorarios "&amp;PROPER(TEXT(B8,"mmmm"))</f>
         <v>#VALUE!</v>
       </c>
       <c r="M8" s="4">
@@ -2322,7 +2322,7 @@
         <v>19000</v>
       </c>
       <c r="O8" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>190082.63099999999</v>
       </c>
       <c r="P8" s="11" t="s">
@@ -2337,44 +2337,44 @@
         <v>2</v>
       </c>
       <c r="V8" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>10.004349</v>
       </c>
       <c r="W8" s="18" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>19000.00</v>
       </c>
       <c r="X8" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y8" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z8" s="1" t="str">
-        <f>TEXT(T8,"DD/MM/YYYY")</f>
+        <f t="shared" si="6"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="AA8" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>39917.35</v>
       </c>
       <c r="AB8" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>229999.98</v>
       </c>
       <c r="AC8" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>190082.63</v>
       </c>
       <c r="AD8" s="10" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0.02</v>
       </c>
       <c r="AE8" s="1"/>
       <c r="AF8" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="AG8" s="15" t="str">
@@ -2382,59 +2382,59 @@
         <v>33615420269-1</v>
       </c>
       <c r="AH8" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI8" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ8" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK8" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AL8" s="2"/>
       <c r="AM8" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>229999.98</v>
       </c>
       <c r="AN8" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>190082.63</v>
       </c>
       <c r="AO8" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>10.004348999999999</v>
       </c>
       <c r="AP8" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>230000</v>
       </c>
       <c r="AQ8" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>10.004348999999999</v>
       </c>
       <c r="AR8" s="2"/>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="17"/>
         <v>45084</v>
       </c>
       <c r="B9" s="9" t="e">
-        <f ca="1">TEXT(DATE(YEAR(C9),MONTH(C9),1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="C9" s="9" t="str">
-        <f ca="1">TEXT(EOMONTH(A9,-1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>31/05/YYYY</v>
       </c>
       <c r="D9" s="9" t="str">
-        <f ca="1">TEXT(A9+14,"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>21/06/YYYY</v>
       </c>
       <c r="E9" s="2">
@@ -2459,7 +2459,7 @@
         <v>57</v>
       </c>
       <c r="L9" s="1" t="e">
-        <f t="shared" ca="1" si="20"/>
+        <f t="shared" ca="1" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="M9" s="4">
@@ -2469,7 +2469,7 @@
         <v>19000</v>
       </c>
       <c r="O9" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19421.477000000003</v>
       </c>
       <c r="P9" s="11" t="s">
@@ -2484,44 +2484,44 @@
         <v>2</v>
       </c>
       <c r="V9" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.022183</v>
       </c>
       <c r="W9" s="18" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>19000.00</v>
       </c>
       <c r="X9" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y9" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z9" s="1" t="str">
-        <f>TEXT(T9,"DD/MM/YYYY")</f>
+        <f t="shared" si="6"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="AA9" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4078.51</v>
       </c>
       <c r="AB9" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>23499.99</v>
       </c>
       <c r="AC9" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>19421.48</v>
       </c>
       <c r="AD9" s="10" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0.01</v>
       </c>
       <c r="AE9" s="1"/>
       <c r="AF9" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="AG9" s="15" t="str">
@@ -2529,59 +2529,59 @@
         <v>20147130202-1</v>
       </c>
       <c r="AH9" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI9" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ9" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK9" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AL9" s="2"/>
       <c r="AM9" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>23499.99</v>
       </c>
       <c r="AN9" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>19421.48</v>
       </c>
       <c r="AO9" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.0221830000000001</v>
       </c>
       <c r="AP9" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>23500</v>
       </c>
       <c r="AQ9" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>1.0221830000000001</v>
       </c>
       <c r="AR9" s="2"/>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="17"/>
         <v>45084</v>
       </c>
       <c r="B10" s="9" t="e">
-        <f ca="1">TEXT(DATE(YEAR(C10),MONTH(C10),1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="C10" s="9" t="str">
-        <f ca="1">TEXT(EOMONTH(A10,-1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>31/05/YYYY</v>
       </c>
       <c r="D10" s="9" t="str">
-        <f ca="1">TEXT(A10+14,"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>21/06/YYYY</v>
       </c>
       <c r="E10" s="2">
@@ -2606,7 +2606,7 @@
         <v>56</v>
       </c>
       <c r="L10" s="1" t="e">
-        <f t="shared" ca="1" si="20"/>
+        <f t="shared" ca="1" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="M10" s="4">
@@ -2616,7 +2616,7 @@
         <v>19000</v>
       </c>
       <c r="O10" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19834.708000000002</v>
       </c>
       <c r="P10" s="11" t="s">
@@ -2631,44 +2631,44 @@
         <v>2</v>
       </c>
       <c r="V10" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.043932</v>
       </c>
       <c r="W10" s="18" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>19000.00</v>
       </c>
       <c r="X10" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y10" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z10" s="1" t="str">
-        <f>TEXT(T10,"DD/MM/YYYY")</f>
+        <f t="shared" si="6"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="AA10" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4165.29</v>
       </c>
       <c r="AB10" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>24000</v>
       </c>
       <c r="AC10" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>19834.71</v>
       </c>
       <c r="AD10" s="10" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
       <c r="AE10" s="1"/>
       <c r="AF10" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="AG10" s="15" t="str">
@@ -2676,59 +2676,59 @@
         <v>20374730429-1</v>
       </c>
       <c r="AH10" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI10" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="AJ10" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK10" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AL10" s="2"/>
       <c r="AM10" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>24000</v>
       </c>
       <c r="AN10" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>19834.71</v>
       </c>
       <c r="AO10" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.0439320000000001</v>
       </c>
       <c r="AP10" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>24000</v>
       </c>
       <c r="AQ10" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>1.0439320000000001</v>
       </c>
       <c r="AR10" s="2"/>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="17"/>
         <v>45084</v>
       </c>
       <c r="B11" s="9" t="e">
-        <f ca="1">TEXT(DATE(YEAR(C11),MONTH(C11),1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="C11" s="9" t="str">
-        <f ca="1">TEXT(EOMONTH(A11,-1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>31/05/YYYY</v>
       </c>
       <c r="D11" s="9" t="str">
-        <f ca="1">TEXT(A11+14,"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>21/06/YYYY</v>
       </c>
       <c r="E11" s="2">
@@ -2753,7 +2753,7 @@
         <v>56</v>
       </c>
       <c r="L11" s="1" t="e">
-        <f t="shared" ca="1" si="20"/>
+        <f t="shared" ca="1" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="M11" s="4">
@@ -2763,7 +2763,7 @@
         <v>10000</v>
       </c>
       <c r="O11" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>13000</v>
       </c>
       <c r="P11" s="11" t="s">
@@ -2778,44 +2778,44 @@
         <v>2</v>
       </c>
       <c r="V11" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.3</v>
       </c>
       <c r="W11" s="18" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>10000.00</v>
       </c>
       <c r="X11" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y11" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z11" s="1" t="str">
-        <f>TEXT(T11,"DD/MM/YYYY")</f>
+        <f t="shared" si="6"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="AA11" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2256.1999999999998</v>
       </c>
       <c r="AB11" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>13000</v>
       </c>
       <c r="AC11" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>13000.00</v>
       </c>
       <c r="AD11" s="10" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
       <c r="AE11" s="1"/>
       <c r="AF11" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="AG11" s="15" t="str">
@@ -2823,59 +2823,59 @@
         <v>37473042-1</v>
       </c>
       <c r="AH11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="AI11" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ11" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>B</v>
       </c>
       <c r="AK11" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AL11" s="2"/>
       <c r="AM11" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>13000</v>
       </c>
       <c r="AN11" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>10743.8</v>
       </c>
       <c r="AO11" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.3</v>
       </c>
       <c r="AP11" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>13000</v>
       </c>
       <c r="AQ11" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>1.3</v>
       </c>
       <c r="AR11" s="2"/>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="17"/>
         <v>45084</v>
       </c>
       <c r="B12" s="9" t="e">
-        <f ca="1">TEXT(DATE(YEAR(C12),MONTH(C12),1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="C12" s="9" t="str">
-        <f ca="1">TEXT(EOMONTH(A12,-1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>31/05/YYYY</v>
       </c>
       <c r="D12" s="9" t="str">
-        <f ca="1">TEXT(A12+14,"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>21/06/YYYY</v>
       </c>
       <c r="E12" s="2">
@@ -2900,7 +2900,7 @@
         <v>60</v>
       </c>
       <c r="L12" s="1" t="e">
-        <f t="shared" ca="1" si="20"/>
+        <f t="shared" ca="1" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="M12" s="4">
@@ -2910,7 +2910,7 @@
         <v>19000</v>
       </c>
       <c r="O12" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>23000</v>
       </c>
       <c r="P12" s="11" t="s">
@@ -2925,44 +2925,44 @@
         <v>2</v>
       </c>
       <c r="V12" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.210526</v>
       </c>
       <c r="W12" s="18" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>19000.00</v>
       </c>
       <c r="X12" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y12" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z12" s="1" t="str">
-        <f>TEXT(T12,"DD/MM/YYYY")</f>
+        <f t="shared" si="6"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="AA12" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3991.74</v>
       </c>
       <c r="AB12" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>23000</v>
       </c>
       <c r="AC12" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>23000.00</v>
       </c>
       <c r="AD12" s="10" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
       <c r="AE12" s="1"/>
       <c r="AF12" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="AG12" s="15" t="str">
@@ -2970,59 +2970,59 @@
         <v>30707354719-1</v>
       </c>
       <c r="AH12" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ12" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>B</v>
       </c>
       <c r="AK12" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AL12" s="2"/>
       <c r="AM12" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>23000</v>
       </c>
       <c r="AN12" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>19008.259999999998</v>
       </c>
       <c r="AO12" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.2105263157894737</v>
       </c>
       <c r="AP12" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>23000</v>
       </c>
       <c r="AQ12" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>1.2105263157894737</v>
       </c>
       <c r="AR12" s="2"/>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="17"/>
         <v>45084</v>
       </c>
       <c r="B13" s="9" t="e">
-        <f ca="1">TEXT(DATE(YEAR(C13),MONTH(C13),1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="C13" s="9" t="str">
-        <f ca="1">TEXT(EOMONTH(A13,-1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>31/05/YYYY</v>
       </c>
       <c r="D13" s="9" t="str">
-        <f ca="1">TEXT(A13+14,"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>21/06/YYYY</v>
       </c>
       <c r="E13" s="2">
@@ -3045,7 +3045,7 @@
         <v>70</v>
       </c>
       <c r="L13" s="1" t="e">
-        <f t="shared" ca="1" si="20"/>
+        <f t="shared" ca="1" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="M13" s="4">
@@ -3055,7 +3055,7 @@
         <v>19000</v>
       </c>
       <c r="O13" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>28500</v>
       </c>
       <c r="P13" s="11"/>
@@ -3068,44 +3068,44 @@
         <v>2</v>
       </c>
       <c r="V13" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
       <c r="W13" s="18" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>19000.00</v>
       </c>
       <c r="X13" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y13" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z13" s="1" t="str">
-        <f>TEXT(T13,"DD/MM/YYYY")</f>
+        <f t="shared" si="6"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="AA13" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB13" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>28500</v>
       </c>
       <c r="AC13" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>28500.00</v>
       </c>
       <c r="AD13" s="10" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
       <c r="AE13" s="1"/>
       <c r="AF13" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="AG13" s="15" t="str">
@@ -3113,59 +3113,59 @@
         <v>-0</v>
       </c>
       <c r="AH13" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI13" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ13" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>C</v>
       </c>
       <c r="AK13" s="1">
-        <f t="shared" si="16"/>
+        <f>IF(LEFT(F13,4)="Nota",0,IF(LEFT(F13,6)="Recibo",2,1))</f>
         <v>1</v>
       </c>
       <c r="AL13" s="2"/>
       <c r="AM13" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>28500</v>
       </c>
       <c r="AN13" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>28500</v>
       </c>
       <c r="AO13" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.5</v>
       </c>
       <c r="AP13" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>28500</v>
       </c>
       <c r="AQ13" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>1.5</v>
       </c>
       <c r="AR13" s="2"/>
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="17"/>
         <v>45084</v>
       </c>
       <c r="B14" s="9" t="e">
-        <f ca="1">TEXT(DATE(YEAR(C14),MONTH(C14),1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="C14" s="9" t="str">
-        <f ca="1">TEXT(EOMONTH(A14,-1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>31/05/YYYY</v>
       </c>
       <c r="D14" s="9" t="str">
-        <f ca="1">TEXT(A14+14,"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>21/06/YYYY</v>
       </c>
       <c r="E14" s="2">
@@ -3199,7 +3199,7 @@
         <v>19000</v>
       </c>
       <c r="O14" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>133471.06700000001</v>
       </c>
       <c r="P14" s="11" t="s">
@@ -3222,44 +3222,44 @@
         <v>2</v>
       </c>
       <c r="V14" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7.024793</v>
       </c>
       <c r="W14" s="18" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>19000.00</v>
       </c>
       <c r="X14" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>00002</v>
       </c>
       <c r="Y14" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>00000150</v>
       </c>
       <c r="Z14" s="1" t="str">
-        <f>TEXT(T14,"DD/MM/YYYY")</f>
+        <f t="shared" si="6"/>
         <v>12/09/YYYY</v>
       </c>
       <c r="AA14" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28028.92</v>
       </c>
       <c r="AB14" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>161499.99</v>
       </c>
       <c r="AC14" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>133471.07</v>
       </c>
       <c r="AD14" s="10" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0.01</v>
       </c>
       <c r="AE14" s="1"/>
       <c r="AF14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="AG14" s="15" t="str">
@@ -3267,59 +3267,59 @@
         <v>30684125792-1</v>
       </c>
       <c r="AH14" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI14" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ14" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK14" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="AK14:AK17" si="25">IF(LEFT(F14,4)="Nota",0,IF(LEFT(F14,6)="Recibo",2,1))</f>
         <v>0</v>
       </c>
       <c r="AL14" s="2"/>
       <c r="AM14" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>161499.99</v>
       </c>
       <c r="AN14" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>133471.07</v>
       </c>
       <c r="AO14" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>7.0247929999999998</v>
       </c>
       <c r="AP14" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>161500</v>
       </c>
       <c r="AQ14" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>7.0247929999999998</v>
       </c>
       <c r="AR14" s="2"/>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="17"/>
         <v>45084</v>
       </c>
       <c r="B15" s="9" t="e">
-        <f ca="1">TEXT(DATE(YEAR(C15),MONTH(C15),1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="C15" s="9" t="str">
-        <f ca="1">TEXT(EOMONTH(A15,-1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>31/05/YYYY</v>
       </c>
       <c r="D15" s="9" t="str">
-        <f ca="1">TEXT(A15+14,"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>21/06/YYYY</v>
       </c>
       <c r="E15" s="2">
@@ -3353,7 +3353,7 @@
         <v>19000</v>
       </c>
       <c r="O15" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>28500</v>
       </c>
       <c r="P15" s="11" t="s">
@@ -3376,44 +3376,44 @@
         <v>2</v>
       </c>
       <c r="V15" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
       <c r="W15" s="18" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>19000.00</v>
       </c>
       <c r="X15" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>00002</v>
       </c>
       <c r="Y15" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>00000152</v>
       </c>
       <c r="Z15" s="1" t="str">
-        <f>TEXT(T15,"DD/MM/YYYY")</f>
+        <f t="shared" si="6"/>
         <v>12/09/YYYY</v>
       </c>
       <c r="AA15" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4946.28</v>
       </c>
       <c r="AB15" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>28500</v>
       </c>
       <c r="AC15" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>28500.00</v>
       </c>
       <c r="AD15" s="10" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
       <c r="AE15" s="1"/>
       <c r="AF15" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="AG15" s="15" t="str">
@@ -3421,59 +3421,59 @@
         <v>30707354719-2</v>
       </c>
       <c r="AH15" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI15" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ15" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>B</v>
       </c>
       <c r="AK15" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="AL15" s="2"/>
       <c r="AM15" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>28500</v>
       </c>
       <c r="AN15" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>23553.72</v>
       </c>
       <c r="AO15" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.5</v>
       </c>
       <c r="AP15" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>28500</v>
       </c>
       <c r="AQ15" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>1.5</v>
       </c>
       <c r="AR15" s="2"/>
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="17"/>
         <v>45084</v>
       </c>
       <c r="B16" s="9" t="e">
-        <f ca="1">TEXT(DATE(YEAR(C16),MONTH(C16),1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="C16" s="9" t="str">
-        <f ca="1">TEXT(EOMONTH(A16,-1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>31/05/YYYY</v>
       </c>
       <c r="D16" s="9" t="str">
-        <f ca="1">TEXT(A16+14,"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>21/06/YYYY</v>
       </c>
       <c r="E16" s="2">
@@ -3507,7 +3507,7 @@
         <v>19000</v>
       </c>
       <c r="O16" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>133057.83600000001</v>
       </c>
       <c r="P16" s="11" t="s">
@@ -3530,44 +3530,44 @@
         <v>2</v>
       </c>
       <c r="V16" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7.003044</v>
       </c>
       <c r="W16" s="18" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>19000.00</v>
       </c>
       <c r="X16" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>00002</v>
       </c>
       <c r="Y16" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>00000151</v>
       </c>
       <c r="Z16" s="1" t="str">
-        <f>TEXT(T16,"DD/MM/YYYY")</f>
+        <f t="shared" si="6"/>
         <v>12/09/YYYY</v>
       </c>
       <c r="AA16" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>27942.15</v>
       </c>
       <c r="AB16" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>160999.99</v>
       </c>
       <c r="AC16" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>133057.84</v>
       </c>
       <c r="AD16" s="10" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0.01</v>
       </c>
       <c r="AE16" s="1"/>
       <c r="AF16" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
       <c r="AG16" s="15" t="str">
@@ -3575,59 +3575,59 @@
         <v>30684125792-2</v>
       </c>
       <c r="AH16" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI16" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ16" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK16" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="AL16" s="2"/>
       <c r="AM16" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>160999.98000000001</v>
       </c>
       <c r="AN16" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>133057.82999999999</v>
       </c>
       <c r="AO16" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>7.003044</v>
       </c>
       <c r="AP16" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>161000</v>
       </c>
       <c r="AQ16" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>7.003044</v>
       </c>
       <c r="AR16" s="2"/>
     </row>
     <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="17"/>
         <v>45084</v>
       </c>
       <c r="B17" s="9" t="e">
-        <f ca="1">TEXT(DATE(YEAR(C17),MONTH(C17),1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="C17" s="9" t="str">
-        <f ca="1">TEXT(EOMONTH(A17,-1),"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="1"/>
         <v>31/05/YYYY</v>
       </c>
       <c r="D17" s="9" t="str">
-        <f ca="1">TEXT(A17+14,"dd/mm/YYYY")</f>
+        <f t="shared" ca="1" si="2"/>
         <v>21/06/YYYY</v>
       </c>
       <c r="E17" s="2">
@@ -3661,7 +3661,7 @@
         <v>19000</v>
       </c>
       <c r="O17" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>28500</v>
       </c>
       <c r="P17" s="11" t="s">
@@ -3684,44 +3684,44 @@
         <v>2</v>
       </c>
       <c r="V17" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
       <c r="W17" s="18" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>19000.00</v>
       </c>
       <c r="X17" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>00002</v>
       </c>
       <c r="Y17" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>00000153</v>
       </c>
       <c r="Z17" s="1" t="str">
-        <f>TEXT(T17,"DD/MM/YYYY")</f>
+        <f t="shared" si="6"/>
         <v>12/09/YYYY</v>
       </c>
       <c r="AA17" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4946.28</v>
       </c>
       <c r="AB17" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>28500</v>
       </c>
       <c r="AC17" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>28500.00</v>
       </c>
       <c r="AD17" s="10" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
       <c r="AE17" s="1"/>
       <c r="AF17" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
       <c r="AG17" s="15" t="str">
@@ -3729,40 +3729,40 @@
         <v>37473042-2</v>
       </c>
       <c r="AH17" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI17" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ17" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>B</v>
       </c>
       <c r="AK17" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="AL17" s="2"/>
       <c r="AM17" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>28500</v>
       </c>
       <c r="AN17" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>23553.72</v>
       </c>
       <c r="AO17" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1.5</v>
       </c>
       <c r="AP17" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>28500</v>
       </c>
       <c r="AQ17" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>1.5</v>
       </c>
       <c r="AR17" s="2"/>

</xml_diff>